<commit_message>
1.5.3 drop need fid column in future.species files; added to documentation
</commit_message>
<xml_diff>
--- a/data/small.xlsx
+++ b/data/small.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianyandell/Documents/Research/ewing/ewing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9B8833-9D4F-4342-ADE4-A8395ED7ABC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50A85CF-4E33-7648-A6CA-5F4576DB2A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35180" yWindow="-1640" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{2A60D24C-DC64-C449-84DD-C019D084A238}"/>
+    <workbookView xWindow="35180" yWindow="-1640" windowWidth="28040" windowHeight="17440" xr2:uid="{2A60D24C-DC64-C449-84DD-C019D084A238}"/>
   </bookViews>
   <sheets>
     <sheet name="organism.features" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="76">
   <si>
     <t>move</t>
   </si>
@@ -85,9 +85,6 @@
     <t>host</t>
   </si>
   <si>
-    <t>DD</t>
-  </si>
-  <si>
     <t>gravid</t>
   </si>
   <si>
@@ -128,9 +125,6 @@
   </si>
   <si>
     <t>current</t>
-  </si>
-  <si>
-    <t>fid</t>
   </si>
   <si>
     <t>time</t>
@@ -654,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8956A585-82A1-4C49-A77C-0D68492FFCAA}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -694,7 +688,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2">
         <v>20</v>
@@ -703,7 +697,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>8</v>
@@ -726,7 +720,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>12</v>
@@ -747,7 +741,7 @@
         <v>2</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>2</v>
@@ -792,44 +786,41 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C74DF95-803E-224B-992D-58497AA9E35E}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -837,140 +828,125 @@
         <v>12</v>
       </c>
       <c r="C2" s="2">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="D2" s="2">
-        <v>55</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="2">
+      <c r="H2" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2">
-        <v>3</v>
+        <v>92</v>
       </c>
       <c r="D3" s="2">
-        <v>92</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="2">
+        <v>17</v>
+      </c>
+      <c r="H3" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2">
-        <v>3</v>
-      </c>
-      <c r="D4" s="2">
         <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="2">
-        <v>4</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2">
-        <v>4</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="2">
+        <v>17</v>
+      </c>
+      <c r="H6" s="2">
         <v>0</v>
       </c>
     </row>
@@ -981,272 +957,245 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20BB9322-7ABE-0243-A308-B15EAB73B9E5}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2">
+        <v>60</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2">
-        <v>60</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="E3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="2">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="2">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="F5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2">
         <v>12</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="2">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2">
-        <v>12</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="2" t="s">
+      <c r="F6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2">
-        <v>2</v>
-      </c>
-      <c r="D6" s="2">
-        <v>12</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2">
-        <v>6</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="C8" s="2">
-        <v>6</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="B9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2">
-        <v>6</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="2">
+        <v>17</v>
+      </c>
+      <c r="H9" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1259,7 +1208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EBC24A-F31B-4D46-863C-6C8374FE545E}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD8"/>
     </sheetView>
   </sheetViews>
@@ -1267,16 +1216,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1315,7 +1264,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
@@ -1332,7 +1281,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2">
         <v>0</v>
@@ -1384,33 +1333,33 @@
         <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -1436,10 +1385,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
@@ -1465,10 +1414,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
@@ -1494,10 +1443,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
@@ -1523,10 +1472,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>3</v>
@@ -1552,13 +1501,13 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D7" s="2">
         <v>5</v>
@@ -1581,13 +1530,13 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
@@ -1628,33 +1577,33 @@
         <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -1680,10 +1629,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
@@ -1709,10 +1658,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
@@ -1738,10 +1687,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
@@ -1767,10 +1716,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>3</v>
@@ -1796,13 +1745,13 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D7" s="2">
         <v>5</v>
@@ -1825,13 +1774,13 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
@@ -1869,30 +1818,30 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -1918,7 +1867,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -1944,7 +1893,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
@@ -1970,7 +1919,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
@@ -1996,7 +1945,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
@@ -2022,7 +1971,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
@@ -2048,7 +1997,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
@@ -2089,13 +2038,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2239,98 +2188,98 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B2" s="2">
         <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B3" s="2">
         <v>200</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B4" s="2">
         <v>52</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B5" s="2">
         <v>70</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B6" s="2">
         <v>75</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B7" s="2">
         <v>85</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B8" s="2">
         <v>90</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B9" s="2">
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>